<commit_message>
Update splitting by speaker
</commit_message>
<xml_diff>
--- a/inputs/politicians/politicians_by_individuals.xlsx
+++ b/inputs/politicians/politicians_by_individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanalexander/Documents/phd/hansard/data/politicians/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanalexander/Documents/phd/hansard/inputs/politicians/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F3FD65-B1BE-294B-9354-6B099BC00E14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2641FE1-EF19-0944-8D1B-3B47F810234D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40040" yWindow="-10340" windowWidth="25740" windowHeight="23240" xr2:uid="{CA0BA94F-DE87-564B-B86A-D7A8F2619401}"/>
+    <workbookView xWindow="-36460" yWindow="1060" windowWidth="25740" windowHeight="23240" xr2:uid="{CA0BA94F-DE87-564B-B86A-D7A8F2619401}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6692" uniqueCount="5146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6693" uniqueCount="5147">
   <si>
     <t>surname</t>
   </si>
@@ -15466,6 +15466,9 @@
   </si>
   <si>
     <t>wasEverPrimeMinister</t>
+  </si>
+  <si>
+    <t>Rick</t>
   </si>
 </sst>
 </file>
@@ -15823,10 +15826,10 @@
   <dimension ref="A1:S1176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="E1158" sqref="E1158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -53550,6 +53553,9 @@
       <c r="D1157" t="s">
         <v>412</v>
       </c>
+      <c r="E1157" t="s">
+        <v>5146</v>
+      </c>
       <c r="H1157" s="2" t="s">
         <v>4478</v>
       </c>

</xml_diff>